<commit_message>
2015 day 6 completed
</commit_message>
<xml_diff>
--- a/aoc2015/inputs/inputs.xlsx
+++ b/aoc2015/inputs/inputs.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="day2" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="day5" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="day6" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2000" uniqueCount="1987">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2300" uniqueCount="2287">
   <si>
     <t xml:space="preserve">3x11x24</t>
   </si>
@@ -5982,6 +5983,906 @@
   </si>
   <si>
     <t xml:space="preserve">yzsmlbnftftgwadz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 660,55 through 986,197</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 341,304 through 638,850</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 199,133 through 461,193</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 322,558 through 977,958</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 537,781 through 687,941</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 226,196 through 599,390</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 240,129 through 703,297</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 317,329 through 451,798</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 957,736 through 977,890</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 263,530 through 559,664</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 158,270 through 243,802</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 223,39 through 454,511</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 544,218 through 979,872</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 313,306 through 363,621</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 173,401 through 496,407</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 333,60 through 748,159</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 87,577 through 484,608</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 809,648 through 826,999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 352,432 through 628,550</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 197,408 through 579,569</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 1,629 through 802,633</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 61,44 through 567,111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 880,25 through 903,973</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 347,123 through 864,746</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 728,877 through 996,975</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 121,895 through 349,906</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 888,547 through 931,628</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 398,782 through 834,882</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 966,850 through 989,953</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 891,543 through 914,991</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 908,77 through 916,117</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 576,900 through 943,934</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 580,170 through 963,206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 184,638 through 192,944</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 940,147 through 978,730</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 854,56 through 965,591</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 717,172 through 947,995</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 426,987 through 705,998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 987,157 through 992,278</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 995,774 through 997,784</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 796,96 through 845,182</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 451,87 through 711,655</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 380,93 through 968,676</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 263,468 through 343,534</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 917,936 through 928,959</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 478,7 through 573,148</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 428,339 through 603,624</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 400,880 through 914,953</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 679,428 through 752,779</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 697,981 through 709,986</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 482,566 through 505,725</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 956,368 through 993,516</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 735,823 through 783,883</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 48,487 through 892,496</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 116,680 through 564,819</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 633,865 through 729,930</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 314,618 through 571,922</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 138,166 through 936,266</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 444,732 through 664,960</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 109,337 through 972,497</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 51,432 through 77,996</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 259,297 through 366,744</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 801,130 through 917,544</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 767,982 through 847,996</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 216,507 through 863,885</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 61,441 through 465,731</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 849,970 through 944,987</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 845,76 through 852,951</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 732,615 through 851,936</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 251,128 through 454,778</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 324,429 through 352,539</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 52,450 through 932,863</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 449,379 through 789,490</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 317,319 through 936,449</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 887,670 through 957,838</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 671,613 through 856,664</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 186,648 through 985,991</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 471,689 through 731,717</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 91,331 through 750,758</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 201,73 through 956,524</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 82,614 through 520,686</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 84,287 through 467,734</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 132,367 through 208,838</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 558,684 through 663,920</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 237,952 through 265,997</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 694,713 through 714,754</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 632,523 through 862,827</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 918,780 through 948,916</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 349,586 through 663,976</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 231,29 through 257,589</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 886,428 through 902,993</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 106,353 through 236,374</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 734,577 through 759,684</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 347,843 through 696,912</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 286,699 through 964,883</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 605,875 through 960,987</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 328,286 through 869,461</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 472,569 through 980,848</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 673,573 through 702,884</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 398,284 through 738,332</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 158,50 through 284,411</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 390,284 through 585,663</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 156,579 through 646,581</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 875,493 through 989,980</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 486,391 through 924,539</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 236,722 through 272,964</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 228,282 through 470,581</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 584,389 through 750,761</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 899,516 through 900,925</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 105,229 through 822,846</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 253,77 through 371,877</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 826,987 through 906,992</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 13,152 through 615,931</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 835,320 through 942,399</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 463,504 through 536,720</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 746,942 through 786,998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 867,333 through 965,403</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 591,477 through 743,692</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 403,437 through 508,908</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 26,723 through 368,814</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 409,485 through 799,809</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 115,630 through 704,705</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 228,183 through 317,220</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 300,649 through 382,842</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 495,365 through 745,562</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 698,346 through 744,873</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 822,932 through 951,934</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 805,30 through 925,421</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 441,152 through 653,274</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 160,81 through 257,587</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 350,781 through 532,917</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 40,583 through 348,636</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 280,306 through 483,395</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 392,936 through 880,955</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 496,591 through 851,934</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 780,887 through 946,994</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 205,735 through 281,863</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 100,876 through 937,915</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 392,393 through 702,878</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 956,374 through 976,636</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 478,262 through 894,775</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 279,65 through 451,677</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 397,541 through 809,847</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 444,291 through 451,586</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 721,408 through 861,598</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 275,365 through 609,382</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 736,24 through 839,72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 86,492 through 582,712</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 676,676 through 709,703</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 105,710 through 374,817</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 328,748 through 845,757</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 335,79 through 394,326</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 193,157 through 633,885</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 227,48 through 769,743</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 148,333 through 614,568</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 22,30 through 436,263</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 547,447 through 688,969</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 576,621 through 987,740</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 711,334 through 799,515</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 541,448 through 654,951</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 792,199 through 798,990</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 89,956 through 609,960</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 724,433 through 929,630</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 144,895 through 201,916</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 226,730 through 632,871</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 760,819 through 828,974</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 887,180 through 940,310</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 222,327 through 805,590</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 630,824 through 885,963</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 940,740 through 954,946</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 193,373 through 779,515</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 304,955 through 469,975</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 405,480 through 546,960</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 662,123 through 690,669</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 615,238 through 750,714</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 423,220 through 930,353</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 329,769 through 358,970</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 590,151 through 704,722</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 884,539 through 894,671</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 449,241 through 984,549</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 449,260 through 496,464</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 306,448 through 602,924</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 286,805 through 555,901</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 722,177 through 922,298</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 491,554 through 723,753</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 80,849 through 174,996</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 296,561 through 530,856</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 653,10 through 972,284</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 529,236 through 672,614</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 791,598 through 989,695</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 19,45 through 575,757</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 111,55 through 880,871</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 197,897 through 943,982</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 912,336 through 977,605</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 101,221 through 537,450</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 101,104 through 969,447</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 71,527 through 587,717</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 336,445 through 593,889</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 214,179 through 575,699</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 86,313 through 96,674</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 566,427 through 906,888</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 641,597 through 850,845</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 606,524 through 883,704</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 835,775 through 867,887</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 547,301 through 897,515</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 289,930 through 413,979</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 361,122 through 457,226</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 162,187 through 374,746</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 348,461 through 454,675</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 966,532 through 985,537</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 172,354 through 630,606</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 501,880 through 680,993</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 8,70 through 566,592</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 433,73 through 690,651</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 840,798 through 902,971</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 822,204 through 893,760</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 453,496 through 649,795</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 969,549 through 990,942</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 789,28 through 930,267</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 880,98 through 932,434</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 568,674 through 669,753</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 686,228 through 903,271</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 263,995 through 478,999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 534,675 through 687,955</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 342,434 through 592,986</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 404,768 through 677,867</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 126,723 through 978,987</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 749,675 through 978,959</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 445,330 through 446,885</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 463,205 through 924,815</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 417,430 through 915,472</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 544,990 through 912,999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 201,255 through 834,789</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 261,142 through 537,862</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 562,934 through 832,984</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 459,978 through 691,980</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 73,911 through 971,972</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 560,448 through 723,810</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 204,630 through 217,854</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 91,259 through 611,607</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 877,32 through 978,815</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 950,438 through 974,746</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 426,30 through 609,917</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 696,37 through 859,201</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 242,417 through 682,572</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 388,401 through 979,528</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 79,345 through 848,685</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 98,91 through 800,434</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 650,700 through 972,843</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 530,450 through 538,926</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 428,559 through 962,909</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 78,138 through 92,940</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 194,117 through 867,157</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 785,355 through 860,617</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 379,441 through 935,708</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 605,133 through 644,911</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 10,963 through 484,975</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 359,988 through 525,991</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 509,138 through 787,411</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 556,467 through 562,773</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 119,486 through 246,900</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 445,561 through 794,673</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 598,681 through 978,921</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 974,230 through 995,641</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 760,75 through 800,275</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 441,215 through 528,680</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 701,636 through 928,877</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 165,753 through 202,780</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 501,412 through 998,516</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 161,105 through 657,395</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 113,340 through 472,972</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 384,994 through 663,999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 969,994 through 983,997</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 519,600 through 750,615</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 363,899 through 948,935</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 271,845 through 454,882</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 376,528 through 779,640</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 767,98 through 854,853</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 107,322 through 378,688</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 235,899 through 818,932</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 445,611 through 532,705</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 629,387 through 814,577</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 112,414 through 387,421</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 319,184 through 382,203</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 627,796 through 973,940</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 602,45 through 763,151</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 441,375 through 974,545</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 871,952 through 989,998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 717,272 through 850,817</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 475,711 through 921,882</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 66,191 through 757,481</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 50,197 through 733,656</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 83,575 through 915,728</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 777,812 through 837,912</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 20,984 through 571,994</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off 446,432 through 458,648</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on 715,871 through 722,890</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 424,675 through 740,862</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 580,592 through 671,900</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle 296,687 through 906,775</t>
   </si>
 </sst>
 </file>
@@ -11115,7 +12016,7 @@
   </sheetPr>
   <dimension ref="A1:A1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -16134,4 +17035,1532 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A300"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43.2"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>1987</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>1988</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>1989</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>1990</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>1991</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>1992</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>1993</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>1996</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>1998</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>2026</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>2027</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>2029</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>2032</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>2034</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>2037</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>2039</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>2042</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>2043</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>2044</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>2045</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>2046</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>2047</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
+        <v>2049</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
+        <v>2051</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
+        <v>2052</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>2053</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
+        <v>2054</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
+        <v>2055</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
+        <v>2056</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
+        <v>2057</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
+        <v>2058</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
+        <v>2059</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="s">
+        <v>2060</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
+        <v>2061</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>2062</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="s">
+        <v>2063</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
+        <v>2064</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
+        <v>2065</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="s">
+        <v>2066</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1" t="s">
+        <v>2067</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="s">
+        <v>2068</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="1" t="s">
+        <v>2069</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="s">
+        <v>2070</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="s">
+        <v>2071</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="s">
+        <v>2072</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="s">
+        <v>2073</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="s">
+        <v>2074</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="s">
+        <v>2076</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="s">
+        <v>2077</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1" t="s">
+        <v>2078</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="1" t="s">
+        <v>2079</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1" t="s">
+        <v>2080</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="1" t="s">
+        <v>2081</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="1" t="s">
+        <v>2082</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="1" t="s">
+        <v>2083</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="1" t="s">
+        <v>2084</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="1" t="s">
+        <v>2085</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="1" t="s">
+        <v>2086</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="1" t="s">
+        <v>2087</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="1" t="s">
+        <v>2088</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="1" t="s">
+        <v>2089</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="1" t="s">
+        <v>2090</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="1" t="s">
+        <v>2091</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="1" t="s">
+        <v>2092</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="1" t="s">
+        <v>2093</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="1" t="s">
+        <v>2094</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="1" t="s">
+        <v>2095</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="1" t="s">
+        <v>2096</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="1" t="s">
+        <v>2097</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="1" t="s">
+        <v>2098</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="1" t="s">
+        <v>2099</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="1" t="s">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="1" t="s">
+        <v>2101</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="1" t="s">
+        <v>2102</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="1" t="s">
+        <v>2103</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="1" t="s">
+        <v>2104</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="1" t="s">
+        <v>2105</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="1" t="s">
+        <v>2106</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="1" t="s">
+        <v>2107</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="1" t="s">
+        <v>2108</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="1" t="s">
+        <v>2109</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="1" t="s">
+        <v>2110</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="1" t="s">
+        <v>2111</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="1" t="s">
+        <v>2112</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="1" t="s">
+        <v>2113</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="1" t="s">
+        <v>2114</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="1" t="s">
+        <v>2115</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="1" t="s">
+        <v>2116</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="1" t="s">
+        <v>2117</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="1" t="s">
+        <v>2118</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="1" t="s">
+        <v>2119</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="1" t="s">
+        <v>2120</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="1" t="s">
+        <v>2121</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="1" t="s">
+        <v>2122</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="1" t="s">
+        <v>2123</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="1" t="s">
+        <v>2124</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="1" t="s">
+        <v>2125</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="1" t="s">
+        <v>2126</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="1" t="s">
+        <v>2127</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="1" t="s">
+        <v>2128</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="1" t="s">
+        <v>2129</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="1" t="s">
+        <v>2130</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="1" t="s">
+        <v>2131</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="1" t="s">
+        <v>2132</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="1" t="s">
+        <v>2133</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="1" t="s">
+        <v>2134</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="1" t="s">
+        <v>2135</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="1" t="s">
+        <v>2136</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="1" t="s">
+        <v>2137</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="1" t="s">
+        <v>2138</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="1" t="s">
+        <v>2139</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="1" t="s">
+        <v>2140</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="1" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="1" t="s">
+        <v>2142</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="1" t="s">
+        <v>2143</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="1" t="s">
+        <v>2144</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="1" t="s">
+        <v>2145</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="1" t="s">
+        <v>2146</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="1" t="s">
+        <v>2147</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="1" t="s">
+        <v>2148</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="1" t="s">
+        <v>2149</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="1" t="s">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="1" t="s">
+        <v>2151</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="1" t="s">
+        <v>2152</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="1" t="s">
+        <v>2153</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="1" t="s">
+        <v>2154</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="1" t="s">
+        <v>2155</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="1" t="s">
+        <v>2156</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="1" t="s">
+        <v>2157</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="1" t="s">
+        <v>2158</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="1" t="s">
+        <v>2159</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="1" t="s">
+        <v>2160</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="1" t="s">
+        <v>2161</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="1" t="s">
+        <v>2162</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="1" t="s">
+        <v>2163</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="1" t="s">
+        <v>2164</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="1" t="s">
+        <v>2165</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="1" t="s">
+        <v>2166</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="1" t="s">
+        <v>2167</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="1" t="s">
+        <v>2168</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="1" t="s">
+        <v>2169</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="1" t="s">
+        <v>2170</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="1" t="s">
+        <v>2171</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="1" t="s">
+        <v>2172</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="1" t="s">
+        <v>2173</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="1" t="s">
+        <v>2174</v>
+      </c>
+    </row>
+    <row r="189" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="1" t="s">
+        <v>2175</v>
+      </c>
+    </row>
+    <row r="190" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="1" t="s">
+        <v>2176</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="1" t="s">
+        <v>2177</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="1" t="s">
+        <v>2178</v>
+      </c>
+    </row>
+    <row r="193" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="1" t="s">
+        <v>2179</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="1" t="s">
+        <v>2180</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="1" t="s">
+        <v>2181</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="1" t="s">
+        <v>2182</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="1" t="s">
+        <v>2183</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="1" t="s">
+        <v>2184</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="1" t="s">
+        <v>2185</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="1" t="s">
+        <v>2186</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="1" t="s">
+        <v>2187</v>
+      </c>
+    </row>
+    <row r="202" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="1" t="s">
+        <v>2188</v>
+      </c>
+    </row>
+    <row r="203" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="1" t="s">
+        <v>2189</v>
+      </c>
+    </row>
+    <row r="204" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="1" t="s">
+        <v>2190</v>
+      </c>
+    </row>
+    <row r="205" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="1" t="s">
+        <v>2191</v>
+      </c>
+    </row>
+    <row r="206" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="1" t="s">
+        <v>2192</v>
+      </c>
+    </row>
+    <row r="207" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="1" t="s">
+        <v>2193</v>
+      </c>
+    </row>
+    <row r="208" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="1" t="s">
+        <v>2194</v>
+      </c>
+    </row>
+    <row r="209" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="1" t="s">
+        <v>2195</v>
+      </c>
+    </row>
+    <row r="210" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="1" t="s">
+        <v>2196</v>
+      </c>
+    </row>
+    <row r="211" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A211" s="1" t="s">
+        <v>2197</v>
+      </c>
+    </row>
+    <row r="212" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="1" t="s">
+        <v>2198</v>
+      </c>
+    </row>
+    <row r="213" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="1" t="s">
+        <v>2199</v>
+      </c>
+    </row>
+    <row r="214" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="1" t="s">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="1" t="s">
+        <v>2201</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="1" t="s">
+        <v>2202</v>
+      </c>
+    </row>
+    <row r="217" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A217" s="1" t="s">
+        <v>2203</v>
+      </c>
+    </row>
+    <row r="218" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A218" s="1" t="s">
+        <v>2204</v>
+      </c>
+    </row>
+    <row r="219" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A219" s="1" t="s">
+        <v>2205</v>
+      </c>
+    </row>
+    <row r="220" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A220" s="1" t="s">
+        <v>2206</v>
+      </c>
+    </row>
+    <row r="221" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="1" t="s">
+        <v>2207</v>
+      </c>
+    </row>
+    <row r="222" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A222" s="1" t="s">
+        <v>2208</v>
+      </c>
+    </row>
+    <row r="223" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A223" s="1" t="s">
+        <v>2209</v>
+      </c>
+    </row>
+    <row r="224" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A224" s="1" t="s">
+        <v>2210</v>
+      </c>
+    </row>
+    <row r="225" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A225" s="1" t="s">
+        <v>2211</v>
+      </c>
+    </row>
+    <row r="226" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A226" s="1" t="s">
+        <v>2212</v>
+      </c>
+    </row>
+    <row r="227" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A227" s="1" t="s">
+        <v>2213</v>
+      </c>
+    </row>
+    <row r="228" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A228" s="1" t="s">
+        <v>2214</v>
+      </c>
+    </row>
+    <row r="229" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A229" s="1" t="s">
+        <v>2215</v>
+      </c>
+    </row>
+    <row r="230" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A230" s="1" t="s">
+        <v>2216</v>
+      </c>
+    </row>
+    <row r="231" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A231" s="1" t="s">
+        <v>2217</v>
+      </c>
+    </row>
+    <row r="232" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A232" s="1" t="s">
+        <v>2218</v>
+      </c>
+    </row>
+    <row r="233" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A233" s="1" t="s">
+        <v>2219</v>
+      </c>
+    </row>
+    <row r="234" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A234" s="1" t="s">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="235" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A235" s="1" t="s">
+        <v>2221</v>
+      </c>
+    </row>
+    <row r="236" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A236" s="1" t="s">
+        <v>2222</v>
+      </c>
+    </row>
+    <row r="237" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A237" s="1" t="s">
+        <v>2223</v>
+      </c>
+    </row>
+    <row r="238" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A238" s="1" t="s">
+        <v>2224</v>
+      </c>
+    </row>
+    <row r="239" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A239" s="1" t="s">
+        <v>2225</v>
+      </c>
+    </row>
+    <row r="240" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A240" s="1" t="s">
+        <v>2226</v>
+      </c>
+    </row>
+    <row r="241" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A241" s="1" t="s">
+        <v>2227</v>
+      </c>
+    </row>
+    <row r="242" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A242" s="1" t="s">
+        <v>2228</v>
+      </c>
+    </row>
+    <row r="243" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A243" s="1" t="s">
+        <v>2229</v>
+      </c>
+    </row>
+    <row r="244" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A244" s="1" t="s">
+        <v>2230</v>
+      </c>
+    </row>
+    <row r="245" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A245" s="1" t="s">
+        <v>2231</v>
+      </c>
+    </row>
+    <row r="246" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A246" s="1" t="s">
+        <v>2232</v>
+      </c>
+    </row>
+    <row r="247" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A247" s="1" t="s">
+        <v>2233</v>
+      </c>
+    </row>
+    <row r="248" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A248" s="1" t="s">
+        <v>2234</v>
+      </c>
+    </row>
+    <row r="249" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A249" s="1" t="s">
+        <v>2235</v>
+      </c>
+    </row>
+    <row r="250" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A250" s="1" t="s">
+        <v>2236</v>
+      </c>
+    </row>
+    <row r="251" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A251" s="1" t="s">
+        <v>2237</v>
+      </c>
+    </row>
+    <row r="252" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A252" s="1" t="s">
+        <v>2238</v>
+      </c>
+    </row>
+    <row r="253" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A253" s="1" t="s">
+        <v>2239</v>
+      </c>
+    </row>
+    <row r="254" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A254" s="1" t="s">
+        <v>2240</v>
+      </c>
+    </row>
+    <row r="255" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A255" s="1" t="s">
+        <v>2241</v>
+      </c>
+    </row>
+    <row r="256" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A256" s="1" t="s">
+        <v>2242</v>
+      </c>
+    </row>
+    <row r="257" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A257" s="1" t="s">
+        <v>2243</v>
+      </c>
+    </row>
+    <row r="258" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A258" s="1" t="s">
+        <v>2244</v>
+      </c>
+    </row>
+    <row r="259" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A259" s="1" t="s">
+        <v>2245</v>
+      </c>
+    </row>
+    <row r="260" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A260" s="1" t="s">
+        <v>2246</v>
+      </c>
+    </row>
+    <row r="261" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A261" s="1" t="s">
+        <v>2247</v>
+      </c>
+    </row>
+    <row r="262" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A262" s="1" t="s">
+        <v>2248</v>
+      </c>
+    </row>
+    <row r="263" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A263" s="1" t="s">
+        <v>2249</v>
+      </c>
+    </row>
+    <row r="264" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A264" s="1" t="s">
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="265" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A265" s="1" t="s">
+        <v>2251</v>
+      </c>
+    </row>
+    <row r="266" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A266" s="1" t="s">
+        <v>2252</v>
+      </c>
+    </row>
+    <row r="267" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A267" s="1" t="s">
+        <v>2253</v>
+      </c>
+    </row>
+    <row r="268" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A268" s="1" t="s">
+        <v>2254</v>
+      </c>
+    </row>
+    <row r="269" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A269" s="1" t="s">
+        <v>2255</v>
+      </c>
+    </row>
+    <row r="270" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A270" s="1" t="s">
+        <v>2256</v>
+      </c>
+    </row>
+    <row r="271" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A271" s="1" t="s">
+        <v>2257</v>
+      </c>
+    </row>
+    <row r="272" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A272" s="1" t="s">
+        <v>2258</v>
+      </c>
+    </row>
+    <row r="273" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A273" s="1" t="s">
+        <v>2259</v>
+      </c>
+    </row>
+    <row r="274" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A274" s="1" t="s">
+        <v>2260</v>
+      </c>
+    </row>
+    <row r="275" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A275" s="1" t="s">
+        <v>2261</v>
+      </c>
+    </row>
+    <row r="276" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A276" s="1" t="s">
+        <v>2262</v>
+      </c>
+    </row>
+    <row r="277" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A277" s="1" t="s">
+        <v>2263</v>
+      </c>
+    </row>
+    <row r="278" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A278" s="1" t="s">
+        <v>2264</v>
+      </c>
+    </row>
+    <row r="279" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A279" s="1" t="s">
+        <v>2265</v>
+      </c>
+    </row>
+    <row r="280" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A280" s="1" t="s">
+        <v>2266</v>
+      </c>
+    </row>
+    <row r="281" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A281" s="1" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="282" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A282" s="1" t="s">
+        <v>2268</v>
+      </c>
+    </row>
+    <row r="283" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A283" s="1" t="s">
+        <v>2269</v>
+      </c>
+    </row>
+    <row r="284" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A284" s="1" t="s">
+        <v>2270</v>
+      </c>
+    </row>
+    <row r="285" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A285" s="1" t="s">
+        <v>2271</v>
+      </c>
+    </row>
+    <row r="286" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A286" s="1" t="s">
+        <v>2272</v>
+      </c>
+    </row>
+    <row r="287" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A287" s="1" t="s">
+        <v>2273</v>
+      </c>
+    </row>
+    <row r="288" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A288" s="1" t="s">
+        <v>2274</v>
+      </c>
+    </row>
+    <row r="289" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A289" s="1" t="s">
+        <v>2275</v>
+      </c>
+    </row>
+    <row r="290" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A290" s="1" t="s">
+        <v>2276</v>
+      </c>
+    </row>
+    <row r="291" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A291" s="1" t="s">
+        <v>2277</v>
+      </c>
+    </row>
+    <row r="292" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A292" s="1" t="s">
+        <v>2278</v>
+      </c>
+    </row>
+    <row r="293" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A293" s="1" t="s">
+        <v>2279</v>
+      </c>
+    </row>
+    <row r="294" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A294" s="1" t="s">
+        <v>2280</v>
+      </c>
+    </row>
+    <row r="295" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A295" s="1" t="s">
+        <v>2281</v>
+      </c>
+    </row>
+    <row r="296" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A296" s="1" t="s">
+        <v>2282</v>
+      </c>
+    </row>
+    <row r="297" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A297" s="1" t="s">
+        <v>2283</v>
+      </c>
+    </row>
+    <row r="298" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A298" s="1" t="s">
+        <v>2284</v>
+      </c>
+    </row>
+    <row r="299" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A299" s="1" t="s">
+        <v>2285</v>
+      </c>
+    </row>
+    <row r="300" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A300" s="1" t="s">
+        <v>2286</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>